<commit_message>
Added new pdf files, refactor:
</commit_message>
<xml_diff>
--- a/data_test/test.xlsx
+++ b/data_test/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_PROGRAMOWANIE\_PROJECTS\PDF\data_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1317F0D9-6E62-4C6D-90F6-4546B06DAB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F586F7D3-A2D4-4A22-B286-3433CC911A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{10DBF30D-4F49-4D77-BBB6-7FFB2DA3B424}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Nazwisko, Imie</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>SOKA BAU?</t>
+  </si>
+  <si>
+    <t>BIS?</t>
+  </si>
+  <si>
+    <t>TUNNEL?</t>
   </si>
 </sst>
 </file>
@@ -525,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F60FC8-F95F-4374-8D7A-8F564EE6F90B}">
-  <dimension ref="A1:I238"/>
+  <dimension ref="A1:K238"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +550,7 @@
     <col min="9" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -566,12 +572,18 @@
       <c r="I1" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -592,8 +604,11 @@
       <c r="H3" s="1">
         <v>44221</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
@@ -614,7 +629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
@@ -635,7 +650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
@@ -652,8 +667,11 @@
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
@@ -674,8 +692,11 @@
       <c r="H7" s="1">
         <v>44221</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -691,49 +712,49 @@
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="F9" s="6"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="F10" s="6"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="F11" s="6"/>
       <c r="G11" s="9"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="F12" s="6"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="F13" s="6"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="F14" s="6"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="F15" s="6"/>
       <c r="G15" s="9"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="F16" s="6"/>
       <c r="G16" s="9"/>

</xml_diff>